<commit_message>
Melhorias no projeto de faturamento, novo gráfico
</commit_message>
<xml_diff>
--- a/Analise_Acumulo_Contas/Geral2014_17.xlsx
+++ b/Analise_Acumulo_Contas/Geral2014_17.xlsx
@@ -870,7 +870,7 @@
         <v>1504357.73</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="29">
@@ -898,7 +898,7 @@
         <v>2701146.85</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="30">
@@ -926,7 +926,7 @@
         <v>1113072.71</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="31">
@@ -945,16 +945,16 @@
         <v>1412245.56</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>5353526.0</v>
+        <v>5353535.0</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>1.1701416624E8</v>
+        <v>1.1701438364E8</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>1412245.56</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="32">
@@ -982,7 +982,7 @@
         <v>2242626.02</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="33">
@@ -1010,7 +1010,7 @@
         <v>1568212.03</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="34">
@@ -1029,16 +1029,16 @@
         <v>2176220.36</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>6092237.0</v>
+        <v>6092265.0</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>1.2508253993E8</v>
+        <v>1.2508612842E8</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>2176220.36</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="35">
@@ -1057,16 +1057,16 @@
         <v>1296098.63</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>6204164.0</v>
+        <v>6204170.0</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>1.2371383107E8</v>
+        <v>1.2371593442E8</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>1296098.63</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="36">
@@ -1085,16 +1085,16 @@
         <v>529974.82</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>5717985.0</v>
+        <v>5718034.0</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>1.2393479829E8</v>
+        <v>1.2395530399E8</v>
       </c>
       <c r="G36" s="1" t="n">
         <v>529974.82</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="37">
@@ -1113,16 +1113,16 @@
         <v>651841.68</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>5690200.0</v>
+        <v>5690223.0</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>1.1398935969E8</v>
+        <v>1.140186704E8</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>651841.68</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="38">
@@ -1141,16 +1141,16 @@
         <v>8767354.29</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>6398510.0</v>
+        <v>6398850.0</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>1.3062837235E8</v>
+        <v>1.3063388688E8</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>8767354.29</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="39">
@@ -1169,16 +1169,16 @@
         <v>2726532.5</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>5379411.0</v>
+        <v>5379442.0</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>1.0799407547E8</v>
+        <v>1.0799527146E8</v>
       </c>
       <c r="G39" s="1" t="n">
         <v>2726532.5</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="40">
@@ -1197,16 +1197,16 @@
         <v>1435164.54</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>6808195.0</v>
+        <v>6817527.0</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>1.4101151979E8</v>
+        <v>1.4120086472E8</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>1435164.54</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="41">
@@ -1225,16 +1225,16 @@
         <v>3995514.67</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>6677496.0</v>
+        <v>6716608.0</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>1.24558838E8</v>
+        <v>1.2589572756E8</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>3995514.67</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="42">
@@ -1253,16 +1253,16 @@
         <v>1003228.13</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>6586693.0</v>
+        <v>7123312.0</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>1.355241881E8</v>
+        <v>1.4255201545E8</v>
       </c>
       <c r="G42" s="1" t="n">
         <v>1003228.13</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="43">
@@ -1281,16 +1281,44 @@
         <v>685550.07</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>2646274.0</v>
+        <v>6199778.0</v>
       </c>
       <c r="F43" s="1" t="n">
-        <v>6.877151152E7</v>
+        <v>1.1781113085E8</v>
       </c>
       <c r="G43" s="1" t="n">
         <v>685550.07</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>201707</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>6967247.0</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>1.2690413221E8</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>2582971.22</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>2828194.0</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>6.924801487E7</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <v>2582971.22</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -1348,7 +1376,7 @@
 group by to_char(DATA_ATENDIMENTO, 'RRRRMM'),
          substr(fc.ID_TEMPO_MES_ANO_REF,1,6),
          1) t
-where    t.anomes between '201401' and '201706'         
+where    t.anomes between '201401' and '201707'         
 group by t.anomes
 having  sum(nvl(t.QTA_FT,0)) + sum(nvl(t.VA_FT,0)) + sum(nvl(t.QTA_AT,0)) + sum(nvl(t.VA_AT,0)) &lt;&gt; 0
 and     substr(t.anomes,1,3) = '201'

</xml_diff>